<commit_message>
fix an incorrect format in A_collection_of_apr_tools.xlsx
</commit_message>
<xml_diff>
--- a/metadata_manager/output/apr_literature_metadata.xlsx
+++ b/metadata_manager/output/apr_literature_metadata.xlsx
@@ -11999,7 +11999,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>['two separate datasets using our\nsingle and dual slicing techniques']</t>
+          <t>['two separate datasets using our single and dual slicing techniques']</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -13192,7 +13192,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>['119 real bugs from open\nsource projects']</t>
+          <t>['119 real bugs from open source projects']</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -14395,7 +14395,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>['5 programs from\nSiemens set of benchmarks with injected faults']</t>
+          <t>['5 programs from Siemens set of benchmarks with injected faults']</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">

</xml_diff>